<commit_message>
coming soon stubs complete
Signed-off-by: Tathagata Chakraborti <tchakra2@outlook.com>
</commit_message>
<xml_diff>
--- a/src/compiler/data/macq-slug.xlsx
+++ b/src/compiler/data/macq-slug.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tchakra2/survey-visualizer/src/compiler/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96DF964-633F-5A4A-8A00-020ECF2BFE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E2497C-2009-6D48-91EA-FDB6A6BE1A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="392">
   <si>
     <t>Slug</t>
   </si>
@@ -1235,6 +1235,9 @@
   </si>
   <si>
     <t>We consider the problem of learning propositional STRIPS world models from action traces alone, using a deep learning architecture (transformers) and gradient descent. The task is cast as a supervised next token prediction problem where the tokens are the actions, and an action a may follow an action sequence if the hidden effects of the previous actions do not make an action precondition of a false. We show that a suitable transformer architecture can faithfully represent propositional STRIPS world models, and that the models can be learned from sets of random valid (positive) and invalid (negative) action sequences alone. A number of experiments are reported.</t>
+  </si>
+  <si>
+    <t>Partial Effects</t>
   </si>
 </sst>
 </file>
@@ -1402,15 +1405,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1633,43 +1636,43 @@
   <dimension ref="A1:AN104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K66" sqref="K66"/>
+      <selection pane="bottomRight" activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:40" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="20" t="s">
@@ -1731,7 +1734,7 @@
       <c r="S2" s="19"/>
       <c r="T2" s="19"/>
       <c r="U2" s="19"/>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="W2" s="19"/>
@@ -1773,13 +1776,13 @@
       </c>
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="Q3" s="19"/>
       <c r="R3" s="19"/>
       <c r="S3" s="19"/>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="U3" s="19"/>
@@ -1807,7 +1810,7 @@
         <v>21</v>
       </c>
       <c r="AK3" s="19"/>
-      <c r="AL3" s="18" t="s">
+      <c r="AL3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AM3" s="19"/>
@@ -1894,7 +1897,7 @@
         <v>39</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>40</v>
+        <v>391</v>
       </c>
       <c r="AI4" s="1" t="s">
         <v>31</v>
@@ -10323,11 +10326,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
     <mergeCell ref="F1:F4"/>
     <mergeCell ref="G1:G4"/>
     <mergeCell ref="K3:L3"/>
@@ -10341,11 +10344,11 @@
     <mergeCell ref="M2:U2"/>
     <mergeCell ref="V2:AN2"/>
     <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -10424,34 +10427,34 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="20" t="s">
@@ -10513,7 +10516,7 @@
       <c r="S2" s="19"/>
       <c r="T2" s="19"/>
       <c r="U2" s="19"/>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="W2" s="19"/>
@@ -10555,13 +10558,13 @@
       </c>
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="Q3" s="19"/>
       <c r="R3" s="19"/>
       <c r="S3" s="19"/>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="U3" s="19"/>
@@ -10589,7 +10592,7 @@
         <v>21</v>
       </c>
       <c r="AK3" s="19"/>
-      <c r="AL3" s="18" t="s">
+      <c r="AL3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AM3" s="19"/>
@@ -18279,11 +18282,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
     <mergeCell ref="F1:F4"/>
     <mergeCell ref="G1:G4"/>
     <mergeCell ref="K3:L3"/>
@@ -18297,11 +18300,11 @@
     <mergeCell ref="M2:U2"/>
     <mergeCell ref="V2:AN2"/>
     <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>